<commit_message>
mydf.key.xlsx re-created by opening mydf.key and keySave as xlsx
</commit_message>
<xml_diff>
--- a/package/kutils/inst/extdata/mydf.key.xlsx
+++ b/package/kutils/inst/extdata/mydf.key.xlsx
@@ -7,13 +7,12 @@
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="varlab" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">name_old</t>
   </si>
@@ -72,19 +71,19 @@
     <t xml:space="preserve">ordered</t>
   </si>
   <si>
-    <t xml:space="preserve">lo&lt;med&lt;hi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lo&lt;mid&lt;mid</t>
+    <t xml:space="preserve">lo&lt;med&lt;hi&lt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lo&lt;mid&lt;mid&lt;.</t>
   </si>
   <si>
     <t xml:space="preserve">x2</t>
   </si>
   <si>
-    <t xml:space="preserve">f|d|c|b|a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f&lt;d&lt;c&lt;b&lt;a</t>
+    <t xml:space="preserve">f|d|c|b|a|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f&lt;d&lt;c&lt;b&lt;a&lt;.</t>
   </si>
   <si>
     <t xml:space="preserve">x1</t>
@@ -93,28 +92,25 @@
     <t xml:space="preserve">factor</t>
   </si>
   <si>
-    <t xml:space="preserve">cindy|bobby|peter|marcia|greg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cindy&lt;Bobby&lt;Peter&lt;Marcia&lt;Greg</t>
+    <t xml:space="preserve">cindy|bobby|peter|marcia|greg|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cindy&lt;Bobby&lt;Peter&lt;Marcia&lt;Greg&lt;.</t>
   </si>
   <si>
     <t xml:space="preserve">x7</t>
   </si>
   <si>
-    <t xml:space="preserve">fail&lt;fail&lt;pass&lt;pass&lt;pass</t>
+    <t xml:space="preserve">fail&lt;fail&lt;pass&lt;pass&lt;pass&lt;.</t>
   </si>
   <si>
     <t xml:space="preserve">x6</t>
   </si>
   <si>
-    <t xml:space="preserve">1|2|3|4|5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F&lt;D&lt;C&lt;B&lt;A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varlab</t>
+    <t xml:space="preserve">1|2|3|4|5|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F&lt;D&lt;C&lt;B&lt;A&lt;.</t>
   </si>
 </sst>
 </file>
@@ -173,17 +169,6 @@
     <tableColumn id="6" name="value_new"/>
     <tableColumn id="7" name="missings"/>
     <tableColumn id="8" name="recodes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B8"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="name_new"/>
-    <tableColumn id="2" name="varlab"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -689,85 +674,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>